<commit_message>
primeras pruebas con lightin
</commit_message>
<xml_diff>
--- a/Data/lighting.xlsx
+++ b/Data/lighting.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F162"/>
+  <dimension ref="A1:J202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +451,37 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Vecino</t>
+          <t>V1L</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Vecino lejano</t>
+          <t>V2L</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Numero jugado</t>
+          <t>V3L</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>V4L</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Acertados</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>No salidos</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Orden</t>
         </is>
       </c>
     </row>
@@ -474,6 +494,10 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -484,6 +508,10 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -494,6 +522,10 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -504,6 +536,10 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -514,6 +550,10 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -524,6 +564,10 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -534,6 +578,10 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -544,6 +592,10 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -554,6 +606,10 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -564,6 +620,10 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -574,6 +634,10 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -584,6 +648,10 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -594,6 +662,10 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -604,6 +676,10 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -614,6 +690,10 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -624,6 +704,10 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -634,6 +718,10 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -644,6 +732,10 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -654,6 +746,10 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -664,6 +760,10 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -674,6 +774,10 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -684,6 +788,10 @@
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -694,6 +802,10 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -704,6 +816,10 @@
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -714,6 +830,10 @@
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -724,6 +844,10 @@
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -734,6 +858,10 @@
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -744,6 +872,10 @@
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -754,6 +886,10 @@
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -764,6 +900,10 @@
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -774,6 +914,10 @@
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -784,6 +928,10 @@
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -794,6 +942,10 @@
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -804,6 +956,10 @@
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -814,6 +970,10 @@
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -824,6 +984,10 @@
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -834,6 +998,10 @@
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -844,6 +1012,10 @@
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -854,6 +1026,10 @@
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -864,6 +1040,10 @@
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -874,6 +1054,10 @@
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -884,6 +1068,10 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -894,6 +1082,10 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -904,6 +1096,10 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -914,6 +1110,10 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -924,6 +1124,10 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -934,6 +1138,10 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -944,6 +1152,10 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -954,6 +1166,10 @@
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -964,6 +1180,10 @@
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -974,6 +1194,10 @@
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -984,6 +1208,10 @@
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -994,6 +1222,10 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1004,6 +1236,10 @@
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1014,6 +1250,10 @@
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1024,6 +1264,10 @@
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1034,6 +1278,10 @@
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1044,6 +1292,10 @@
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1054,6 +1306,10 @@
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1064,6 +1320,10 @@
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -1074,6 +1334,10 @@
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1084,6 +1348,10 @@
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -1094,6 +1362,10 @@
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -1104,6 +1376,10 @@
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1114,6 +1390,10 @@
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1124,6 +1404,10 @@
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -1134,6 +1418,10 @@
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -1144,6 +1432,10 @@
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -1154,6 +1446,10 @@
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -1164,6 +1460,10 @@
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -1174,6 +1474,10 @@
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -1184,6 +1488,10 @@
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -1194,6 +1502,10 @@
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -1204,6 +1516,10 @@
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -1214,6 +1530,10 @@
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -1224,6 +1544,10 @@
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -1234,6 +1558,10 @@
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -1244,6 +1572,10 @@
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -1254,6 +1586,10 @@
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -1264,6 +1600,10 @@
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -1274,6 +1614,10 @@
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -1284,6 +1628,10 @@
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -1294,6 +1642,10 @@
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -1304,6 +1656,10 @@
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -1314,6 +1670,10 @@
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -1324,6 +1684,10 @@
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -1334,6 +1698,10 @@
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -1344,6 +1712,10 @@
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -1354,6 +1726,10 @@
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -1364,6 +1740,10 @@
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -1374,6 +1754,10 @@
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -1384,6 +1768,10 @@
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -1394,6 +1782,10 @@
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr"/>
       <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -1404,6 +1796,10 @@
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -1414,6 +1810,10 @@
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
+      <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -1424,6 +1824,10 @@
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
       <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -1434,6 +1838,10 @@
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
       <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -1444,6 +1852,10 @@
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
       <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -1454,6 +1866,10 @@
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr"/>
       <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -1464,6 +1880,10 @@
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -1474,6 +1894,10 @@
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -1484,6 +1908,10 @@
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -1494,6 +1922,10 @@
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr"/>
       <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr"/>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -1504,6 +1936,10 @@
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr"/>
       <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr"/>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -1514,6 +1950,10 @@
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr"/>
       <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -1524,6 +1964,10 @@
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr"/>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -1534,6 +1978,10 @@
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
       <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr"/>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -1544,6 +1992,10 @@
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr"/>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -1554,6 +2006,10 @@
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
       <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr"/>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -1564,6 +2020,10 @@
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
       <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -1574,6 +2034,10 @@
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -1584,6 +2048,10 @@
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -1594,6 +2062,10 @@
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
       <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -1604,6 +2076,10 @@
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -1614,6 +2090,10 @@
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
       <c r="F116" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -1624,6 +2104,10 @@
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
       <c r="F117" t="inlineStr"/>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -1634,6 +2118,10 @@
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -1644,6 +2132,10 @@
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr"/>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -1654,6 +2146,10 @@
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr"/>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -1664,6 +2160,10 @@
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr"/>
       <c r="F121" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr"/>
+      <c r="I121" t="inlineStr"/>
+      <c r="J121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -1674,6 +2174,10 @@
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
       <c r="F122" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -1684,6 +2188,10 @@
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
       <c r="F123" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr"/>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -1694,6 +2202,10 @@
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr"/>
       <c r="F124" t="inlineStr"/>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -1704,6 +2216,10 @@
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr"/>
       <c r="F125" t="inlineStr"/>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" t="inlineStr"/>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -1714,6 +2230,10 @@
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="inlineStr"/>
       <c r="F126" t="inlineStr"/>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" t="inlineStr"/>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -1724,6 +2244,10 @@
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr"/>
       <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -1734,6 +2258,10 @@
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr"/>
       <c r="F128" t="inlineStr"/>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="inlineStr"/>
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -1744,6 +2272,10 @@
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
       <c r="F129" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -1754,6 +2286,10 @@
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
       <c r="F130" t="inlineStr"/>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="inlineStr"/>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -1764,6 +2300,10 @@
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" t="inlineStr"/>
+      <c r="I131" t="inlineStr"/>
+      <c r="J131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -1774,6 +2314,10 @@
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" t="inlineStr"/>
+      <c r="I132" t="inlineStr"/>
+      <c r="J132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -1784,6 +2328,10 @@
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr"/>
       <c r="F133" t="inlineStr"/>
+      <c r="G133" t="inlineStr"/>
+      <c r="H133" t="inlineStr"/>
+      <c r="I133" t="inlineStr"/>
+      <c r="J133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -1794,6 +2342,10 @@
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr"/>
       <c r="F134" t="inlineStr"/>
+      <c r="G134" t="inlineStr"/>
+      <c r="H134" t="inlineStr"/>
+      <c r="I134" t="inlineStr"/>
+      <c r="J134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -1804,6 +2356,10 @@
       <c r="D135" t="inlineStr"/>
       <c r="E135" t="inlineStr"/>
       <c r="F135" t="inlineStr"/>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" t="inlineStr"/>
+      <c r="I135" t="inlineStr"/>
+      <c r="J135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -1814,6 +2370,10 @@
       <c r="D136" t="inlineStr"/>
       <c r="E136" t="inlineStr"/>
       <c r="F136" t="inlineStr"/>
+      <c r="G136" t="inlineStr"/>
+      <c r="H136" t="inlineStr"/>
+      <c r="I136" t="inlineStr"/>
+      <c r="J136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -1824,6 +2384,10 @@
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="inlineStr"/>
       <c r="F137" t="inlineStr"/>
+      <c r="G137" t="inlineStr"/>
+      <c r="H137" t="inlineStr"/>
+      <c r="I137" t="inlineStr"/>
+      <c r="J137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -1834,6 +2398,10 @@
       <c r="D138" t="inlineStr"/>
       <c r="E138" t="inlineStr"/>
       <c r="F138" t="inlineStr"/>
+      <c r="G138" t="inlineStr"/>
+      <c r="H138" t="inlineStr"/>
+      <c r="I138" t="inlineStr"/>
+      <c r="J138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -1844,6 +2412,10 @@
       <c r="D139" t="inlineStr"/>
       <c r="E139" t="inlineStr"/>
       <c r="F139" t="inlineStr"/>
+      <c r="G139" t="inlineStr"/>
+      <c r="H139" t="inlineStr"/>
+      <c r="I139" t="inlineStr"/>
+      <c r="J139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -1854,6 +2426,10 @@
       <c r="D140" t="inlineStr"/>
       <c r="E140" t="inlineStr"/>
       <c r="F140" t="inlineStr"/>
+      <c r="G140" t="inlineStr"/>
+      <c r="H140" t="inlineStr"/>
+      <c r="I140" t="inlineStr"/>
+      <c r="J140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -1864,6 +2440,10 @@
       <c r="D141" t="inlineStr"/>
       <c r="E141" t="inlineStr"/>
       <c r="F141" t="inlineStr"/>
+      <c r="G141" t="inlineStr"/>
+      <c r="H141" t="inlineStr"/>
+      <c r="I141" t="inlineStr"/>
+      <c r="J141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -1877,9 +2457,11 @@
       <c r="C142" t="inlineStr"/>
       <c r="D142" t="inlineStr"/>
       <c r="E142" t="inlineStr"/>
-      <c r="F142" t="n">
-        <v>1</v>
-      </c>
+      <c r="F142" t="inlineStr"/>
+      <c r="G142" t="inlineStr"/>
+      <c r="H142" t="inlineStr"/>
+      <c r="I142" t="inlineStr"/>
+      <c r="J142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -1893,9 +2475,11 @@
       <c r="C143" t="inlineStr"/>
       <c r="D143" t="inlineStr"/>
       <c r="E143" t="inlineStr"/>
-      <c r="F143" t="n">
-        <v>2</v>
-      </c>
+      <c r="F143" t="inlineStr"/>
+      <c r="G143" t="inlineStr"/>
+      <c r="H143" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
+      <c r="J143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -1909,9 +2493,11 @@
       <c r="C144" t="inlineStr"/>
       <c r="D144" t="inlineStr"/>
       <c r="E144" t="inlineStr"/>
-      <c r="F144" t="n">
-        <v>3</v>
-      </c>
+      <c r="F144" t="inlineStr"/>
+      <c r="G144" t="inlineStr"/>
+      <c r="H144" t="inlineStr"/>
+      <c r="I144" t="inlineStr"/>
+      <c r="J144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -1925,9 +2511,11 @@
       <c r="C145" t="inlineStr"/>
       <c r="D145" t="inlineStr"/>
       <c r="E145" t="inlineStr"/>
-      <c r="F145" t="n">
-        <v>4</v>
-      </c>
+      <c r="F145" t="inlineStr"/>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" t="inlineStr"/>
+      <c r="I145" t="inlineStr"/>
+      <c r="J145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -1941,9 +2529,11 @@
       <c r="C146" t="inlineStr"/>
       <c r="D146" t="inlineStr"/>
       <c r="E146" t="inlineStr"/>
-      <c r="F146" t="n">
-        <v>5</v>
-      </c>
+      <c r="F146" t="inlineStr"/>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr"/>
+      <c r="I146" t="inlineStr"/>
+      <c r="J146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -1957,9 +2547,11 @@
       <c r="C147" t="inlineStr"/>
       <c r="D147" t="inlineStr"/>
       <c r="E147" t="inlineStr"/>
-      <c r="F147" t="n">
-        <v>6</v>
-      </c>
+      <c r="F147" t="inlineStr"/>
+      <c r="G147" t="inlineStr"/>
+      <c r="H147" t="inlineStr"/>
+      <c r="I147" t="inlineStr"/>
+      <c r="J147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -1973,9 +2565,11 @@
       <c r="C148" t="inlineStr"/>
       <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr"/>
-      <c r="F148" t="n">
-        <v>7</v>
-      </c>
+      <c r="F148" t="inlineStr"/>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" t="inlineStr"/>
+      <c r="I148" t="inlineStr"/>
+      <c r="J148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -1989,9 +2583,11 @@
       <c r="C149" t="inlineStr"/>
       <c r="D149" t="inlineStr"/>
       <c r="E149" t="inlineStr"/>
-      <c r="F149" t="n">
-        <v>8</v>
-      </c>
+      <c r="F149" t="inlineStr"/>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" t="inlineStr"/>
+      <c r="I149" t="inlineStr"/>
+      <c r="J149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -2005,9 +2601,11 @@
       <c r="C150" t="inlineStr"/>
       <c r="D150" t="inlineStr"/>
       <c r="E150" t="inlineStr"/>
-      <c r="F150" t="n">
-        <v>9</v>
-      </c>
+      <c r="F150" t="inlineStr"/>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="inlineStr"/>
+      <c r="I150" t="inlineStr"/>
+      <c r="J150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -2021,9 +2619,11 @@
       <c r="C151" t="inlineStr"/>
       <c r="D151" t="inlineStr"/>
       <c r="E151" t="inlineStr"/>
-      <c r="F151" t="n">
-        <v>10</v>
-      </c>
+      <c r="F151" t="inlineStr"/>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -2037,9 +2637,11 @@
       <c r="C152" t="inlineStr"/>
       <c r="D152" t="inlineStr"/>
       <c r="E152" t="inlineStr"/>
-      <c r="F152" t="n">
-        <v>11</v>
-      </c>
+      <c r="F152" t="inlineStr"/>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -2053,9 +2655,11 @@
       <c r="C153" t="inlineStr"/>
       <c r="D153" t="inlineStr"/>
       <c r="E153" t="inlineStr"/>
-      <c r="F153" t="n">
-        <v>12</v>
-      </c>
+      <c r="F153" t="inlineStr"/>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -2069,9 +2673,11 @@
       <c r="C154" t="inlineStr"/>
       <c r="D154" t="inlineStr"/>
       <c r="E154" t="inlineStr"/>
-      <c r="F154" t="n">
-        <v>13</v>
-      </c>
+      <c r="F154" t="inlineStr"/>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr"/>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -2085,9 +2691,11 @@
       <c r="C155" t="inlineStr"/>
       <c r="D155" t="inlineStr"/>
       <c r="E155" t="inlineStr"/>
-      <c r="F155" t="n">
-        <v>14</v>
-      </c>
+      <c r="F155" t="inlineStr"/>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="inlineStr"/>
+      <c r="I155" t="inlineStr"/>
+      <c r="J155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -2101,9 +2709,11 @@
       <c r="C156" t="inlineStr"/>
       <c r="D156" t="inlineStr"/>
       <c r="E156" t="inlineStr"/>
-      <c r="F156" t="n">
-        <v>15</v>
-      </c>
+      <c r="F156" t="inlineStr"/>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="inlineStr"/>
+      <c r="I156" t="inlineStr"/>
+      <c r="J156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -2117,9 +2727,11 @@
       <c r="C157" t="inlineStr"/>
       <c r="D157" t="inlineStr"/>
       <c r="E157" t="inlineStr"/>
-      <c r="F157" t="n">
-        <v>16</v>
-      </c>
+      <c r="F157" t="inlineStr"/>
+      <c r="G157" t="inlineStr"/>
+      <c r="H157" t="inlineStr"/>
+      <c r="I157" t="inlineStr"/>
+      <c r="J157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -2133,9 +2745,11 @@
       <c r="C158" t="inlineStr"/>
       <c r="D158" t="inlineStr"/>
       <c r="E158" t="inlineStr"/>
-      <c r="F158" t="n">
-        <v>17</v>
-      </c>
+      <c r="F158" t="inlineStr"/>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" t="inlineStr"/>
+      <c r="I158" t="inlineStr"/>
+      <c r="J158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -2149,9 +2763,11 @@
       <c r="C159" t="inlineStr"/>
       <c r="D159" t="inlineStr"/>
       <c r="E159" t="inlineStr"/>
-      <c r="F159" t="n">
-        <v>18</v>
-      </c>
+      <c r="F159" t="inlineStr"/>
+      <c r="G159" t="inlineStr"/>
+      <c r="H159" t="inlineStr"/>
+      <c r="I159" t="inlineStr"/>
+      <c r="J159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -2165,9 +2781,11 @@
       <c r="C160" t="inlineStr"/>
       <c r="D160" t="inlineStr"/>
       <c r="E160" t="inlineStr"/>
-      <c r="F160" t="n">
-        <v>19</v>
-      </c>
+      <c r="F160" t="inlineStr"/>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" t="inlineStr"/>
+      <c r="I160" t="inlineStr"/>
+      <c r="J160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -2181,9 +2799,11 @@
       <c r="C161" t="inlineStr"/>
       <c r="D161" t="inlineStr"/>
       <c r="E161" t="inlineStr"/>
-      <c r="F161" t="n">
-        <v>20</v>
-      </c>
+      <c r="F161" t="inlineStr"/>
+      <c r="G161" t="inlineStr"/>
+      <c r="H161" t="inlineStr"/>
+      <c r="I161" t="inlineStr"/>
+      <c r="J161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -2197,8 +2817,1154 @@
       <c r="C162" t="inlineStr"/>
       <c r="D162" t="inlineStr"/>
       <c r="E162" t="inlineStr"/>
-      <c r="F162" t="n">
+      <c r="F162" t="inlineStr"/>
+      <c r="G162" t="inlineStr"/>
+      <c r="H162" t="inlineStr"/>
+      <c r="I162" t="inlineStr"/>
+      <c r="J162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>14</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr"/>
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" t="inlineStr"/>
+      <c r="G163" t="inlineStr"/>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J163" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>12</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
+      <c r="E164" t="inlineStr"/>
+      <c r="F164" t="inlineStr"/>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J164" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>31</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr"/>
+      <c r="F165" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J165" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>25</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr"/>
+      <c r="F166" t="inlineStr"/>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J166" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>7</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
+      <c r="E167" t="inlineStr"/>
+      <c r="F167" t="inlineStr"/>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J167" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>16</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
+      <c r="E168" t="inlineStr"/>
+      <c r="F168" t="inlineStr"/>
+      <c r="G168" t="inlineStr"/>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J168" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>16</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
+      <c r="E169" t="inlineStr"/>
+      <c r="F169" t="inlineStr"/>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J169" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>14</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>{13: 0}</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
+      <c r="E170" t="inlineStr"/>
+      <c r="F170" t="inlineStr"/>
+      <c r="G170" t="inlineStr"/>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J170" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>31</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>{13: 1, 35: 0}</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
+      <c r="E171" t="inlineStr"/>
+      <c r="F171" t="inlineStr"/>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>V4L</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J171" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>17</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>{35: 1}</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
+      <c r="E172" t="inlineStr"/>
+      <c r="F172" t="inlineStr"/>
+      <c r="G172" t="inlineStr"/>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>[13]</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J172" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>14</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>{19: 0, 35: 2}</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
+      <c r="E173" t="inlineStr"/>
+      <c r="F173" t="inlineStr"/>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>V4L</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J173" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>25</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>{35: 3}</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr"/>
+      <c r="D174" t="inlineStr"/>
+      <c r="E174" t="inlineStr"/>
+      <c r="F174" t="inlineStr"/>
+      <c r="G174" t="inlineStr"/>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>[19]</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J174" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>14</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>{35: 4}</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr"/>
+      <c r="D175" t="inlineStr"/>
+      <c r="E175" t="inlineStr"/>
+      <c r="F175" t="inlineStr"/>
+      <c r="G175" t="inlineStr"/>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J175" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>15</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>{35: 5}</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr"/>
+      <c r="D176" t="inlineStr"/>
+      <c r="E176" t="inlineStr"/>
+      <c r="F176" t="inlineStr"/>
+      <c r="G176" t="inlineStr"/>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J176" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>14</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>{35: 6}</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr"/>
+      <c r="D177" t="inlineStr"/>
+      <c r="E177" t="inlineStr"/>
+      <c r="F177" t="inlineStr"/>
+      <c r="G177" t="inlineStr"/>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J177" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>1</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr"/>
+      <c r="D178" t="inlineStr"/>
+      <c r="E178" t="inlineStr"/>
+      <c r="F178" t="inlineStr"/>
+      <c r="G178" t="inlineStr"/>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>[35]</t>
+        </is>
+      </c>
+      <c r="J178" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>9</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr"/>
+      <c r="D179" t="inlineStr"/>
+      <c r="E179" t="inlineStr"/>
+      <c r="F179" t="inlineStr"/>
+      <c r="G179" t="inlineStr"/>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J179" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>32</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr"/>
+      <c r="D180" t="inlineStr"/>
+      <c r="E180" t="inlineStr"/>
+      <c r="F180" t="inlineStr"/>
+      <c r="G180" t="inlineStr"/>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J180" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>12</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>{13: 0}</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr"/>
+      <c r="D181" t="inlineStr"/>
+      <c r="E181" t="inlineStr"/>
+      <c r="F181" t="inlineStr"/>
+      <c r="G181" t="inlineStr"/>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J181" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>20</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>{13: 1}</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr"/>
+      <c r="D182" t="inlineStr"/>
+      <c r="E182" t="inlineStr"/>
+      <c r="F182" t="inlineStr"/>
+      <c r="G182" t="inlineStr"/>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J182" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>10</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>{13: 2}</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr"/>
+      <c r="D183" t="inlineStr"/>
+      <c r="E183" t="inlineStr"/>
+      <c r="F183" t="inlineStr"/>
+      <c r="G183" t="inlineStr"/>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J183" t="n">
         <v>21</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>35</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>{13: 3}</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr"/>
+      <c r="D184" t="inlineStr"/>
+      <c r="E184" t="inlineStr"/>
+      <c r="F184" t="inlineStr"/>
+      <c r="G184" t="inlineStr"/>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J184" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>23</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>{13: 4, 27: 0}</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr"/>
+      <c r="D185" t="inlineStr"/>
+      <c r="E185" t="inlineStr"/>
+      <c r="F185" t="inlineStr"/>
+      <c r="G185" t="inlineStr"/>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J185" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>21</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>{13: 5, 27: 1}</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr"/>
+      <c r="D186" t="inlineStr"/>
+      <c r="E186" t="inlineStr"/>
+      <c r="F186" t="inlineStr"/>
+      <c r="G186" t="inlineStr"/>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J186" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>28</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>{13: 6, 27: 2}</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr"/>
+      <c r="D187" t="inlineStr"/>
+      <c r="E187" t="inlineStr"/>
+      <c r="F187" t="inlineStr"/>
+      <c r="G187" t="inlineStr"/>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J187" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>12</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>{27: 3}</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr"/>
+      <c r="D188" t="inlineStr"/>
+      <c r="E188" t="inlineStr"/>
+      <c r="F188" t="inlineStr"/>
+      <c r="G188" t="inlineStr"/>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>[13]</t>
+        </is>
+      </c>
+      <c r="J188" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>10</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>{27: 4}</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr"/>
+      <c r="D189" t="inlineStr"/>
+      <c r="E189" t="inlineStr"/>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>V3L</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr"/>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J189" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>11</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr"/>
+      <c r="D190" t="inlineStr"/>
+      <c r="E190" t="inlineStr"/>
+      <c r="F190" t="inlineStr"/>
+      <c r="G190" t="inlineStr"/>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>[27]</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J190" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>21</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>{36: 0}</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr"/>
+      <c r="D191" t="inlineStr"/>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>V2L</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr"/>
+      <c r="G191" t="inlineStr"/>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J191" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>27</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr"/>
+      <c r="D192" t="inlineStr"/>
+      <c r="E192" t="inlineStr"/>
+      <c r="F192" t="inlineStr"/>
+      <c r="G192" t="inlineStr"/>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>[36]</t>
+        </is>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J192" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>1</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr"/>
+      <c r="D193" t="inlineStr"/>
+      <c r="E193" t="inlineStr"/>
+      <c r="F193" t="inlineStr"/>
+      <c r="G193" t="inlineStr"/>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J193" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>29</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr"/>
+      <c r="D194" t="inlineStr"/>
+      <c r="E194" t="inlineStr"/>
+      <c r="F194" t="inlineStr"/>
+      <c r="G194" t="inlineStr"/>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J194" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>36</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>{19: 0}</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr"/>
+      <c r="D195" t="inlineStr"/>
+      <c r="E195" t="inlineStr"/>
+      <c r="F195" t="inlineStr"/>
+      <c r="G195" t="inlineStr"/>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J195" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>36</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>{19: 1}</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr"/>
+      <c r="D196" t="inlineStr"/>
+      <c r="E196" t="inlineStr"/>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>V3L</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr"/>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J196" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>2</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>{14: 0}</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr"/>
+      <c r="D197" t="inlineStr"/>
+      <c r="E197" t="inlineStr"/>
+      <c r="F197" t="inlineStr"/>
+      <c r="G197" t="inlineStr"/>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>[19]</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J197" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>5</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>{14: 1}</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr"/>
+      <c r="D198" t="inlineStr"/>
+      <c r="E198" t="inlineStr"/>
+      <c r="F198" t="inlineStr"/>
+      <c r="G198" t="inlineStr"/>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J198" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>15</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>{14: 2}</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr"/>
+      <c r="D199" t="inlineStr"/>
+      <c r="E199" t="inlineStr"/>
+      <c r="F199" t="inlineStr"/>
+      <c r="G199" t="inlineStr"/>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J199" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>32</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>{14: 3}</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr"/>
+      <c r="D200" t="inlineStr"/>
+      <c r="E200" t="inlineStr"/>
+      <c r="F200" t="inlineStr"/>
+      <c r="G200" t="inlineStr"/>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J200" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>11</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>{14: 4}</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr"/>
+      <c r="E201" t="inlineStr"/>
+      <c r="F201" t="inlineStr"/>
+      <c r="G201" t="inlineStr"/>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J201" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>14</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>{24: 0}</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr"/>
+      <c r="D202" t="inlineStr"/>
+      <c r="E202" t="inlineStr"/>
+      <c r="F202" t="inlineStr"/>
+      <c r="G202" t="inlineStr"/>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>[14]</t>
+        </is>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J202" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se volvio hacer bombay1
</commit_message>
<xml_diff>
--- a/Data/lighting.xlsx
+++ b/Data/lighting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\OneDrive\Escritorio\Repositorio\jonatha1992\Predictor_ruleta\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69881850-DE2F-42CA-946C-F96FF90A3B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B57DAA-3C08-409F-BB37-5ADA210A8CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2892" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Salidos" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
ultimos datos de lighting
</commit_message>
<xml_diff>
--- a/Data/lighting.xlsx
+++ b/Data/lighting.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J276"/>
+  <dimension ref="A1:J430"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8217,6 +8217,4318 @@
         <v>133</v>
       </c>
     </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>10</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr"/>
+      <c r="D277" t="inlineStr"/>
+      <c r="E277" t="inlineStr"/>
+      <c r="F277" t="inlineStr"/>
+      <c r="G277" t="inlineStr"/>
+      <c r="H277" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I277" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J277" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>1</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr"/>
+      <c r="D278" t="inlineStr"/>
+      <c r="E278" t="inlineStr"/>
+      <c r="F278" t="inlineStr"/>
+      <c r="G278" t="inlineStr"/>
+      <c r="H278" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I278" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J278" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>24</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr"/>
+      <c r="D279" t="inlineStr"/>
+      <c r="E279" t="inlineStr"/>
+      <c r="F279" t="inlineStr"/>
+      <c r="G279" t="inlineStr"/>
+      <c r="H279" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I279" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J279" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>1</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr"/>
+      <c r="D280" t="inlineStr"/>
+      <c r="E280" t="inlineStr"/>
+      <c r="F280" t="inlineStr"/>
+      <c r="G280" t="inlineStr"/>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J280" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>17</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr"/>
+      <c r="D281" t="inlineStr"/>
+      <c r="E281" t="inlineStr"/>
+      <c r="F281" t="inlineStr"/>
+      <c r="G281" t="inlineStr"/>
+      <c r="H281" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I281" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J281" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>32</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr"/>
+      <c r="D282" t="inlineStr"/>
+      <c r="E282" t="inlineStr"/>
+      <c r="F282" t="inlineStr"/>
+      <c r="G282" t="inlineStr"/>
+      <c r="H282" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I282" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J282" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>17</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr"/>
+      <c r="D283" t="inlineStr"/>
+      <c r="E283" t="inlineStr"/>
+      <c r="F283" t="inlineStr"/>
+      <c r="G283" t="inlineStr"/>
+      <c r="H283" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I283" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J283" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>32</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr"/>
+      <c r="D284" t="inlineStr"/>
+      <c r="E284" t="inlineStr"/>
+      <c r="F284" t="inlineStr"/>
+      <c r="G284" t="inlineStr"/>
+      <c r="H284" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I284" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J284" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>15</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr"/>
+      <c r="D285" t="inlineStr"/>
+      <c r="E285" t="inlineStr"/>
+      <c r="F285" t="inlineStr"/>
+      <c r="G285" t="inlineStr"/>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I285" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J285" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>11</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr"/>
+      <c r="D286" t="inlineStr"/>
+      <c r="E286" t="inlineStr"/>
+      <c r="F286" t="inlineStr"/>
+      <c r="G286" t="inlineStr"/>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I286" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J286" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>13</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr"/>
+      <c r="D287" t="inlineStr"/>
+      <c r="E287" t="inlineStr"/>
+      <c r="F287" t="inlineStr"/>
+      <c r="G287" t="inlineStr"/>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I287" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J287" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>36</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr"/>
+      <c r="D288" t="inlineStr"/>
+      <c r="E288" t="inlineStr"/>
+      <c r="F288" t="inlineStr"/>
+      <c r="G288" t="inlineStr"/>
+      <c r="H288" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I288" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J288" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>20</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr"/>
+      <c r="D289" t="inlineStr"/>
+      <c r="E289" t="inlineStr"/>
+      <c r="F289" t="inlineStr"/>
+      <c r="G289" t="inlineStr"/>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I289" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J289" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>23</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr"/>
+      <c r="D290" t="inlineStr"/>
+      <c r="E290" t="inlineStr"/>
+      <c r="F290" t="inlineStr"/>
+      <c r="G290" t="inlineStr"/>
+      <c r="H290" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I290" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J290" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>10</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr"/>
+      <c r="D291" t="inlineStr"/>
+      <c r="E291" t="inlineStr"/>
+      <c r="F291" t="inlineStr"/>
+      <c r="G291" t="inlineStr"/>
+      <c r="H291" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I291" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J291" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>10</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr"/>
+      <c r="D292" t="inlineStr"/>
+      <c r="E292" t="inlineStr"/>
+      <c r="F292" t="inlineStr"/>
+      <c r="G292" t="inlineStr"/>
+      <c r="H292" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I292" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J292" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>31</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr"/>
+      <c r="D293" t="inlineStr"/>
+      <c r="E293" t="inlineStr"/>
+      <c r="F293" t="inlineStr"/>
+      <c r="G293" t="inlineStr"/>
+      <c r="H293" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I293" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J293" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>14</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr"/>
+      <c r="D294" t="inlineStr"/>
+      <c r="E294" t="inlineStr"/>
+      <c r="F294" t="inlineStr"/>
+      <c r="G294" t="inlineStr"/>
+      <c r="H294" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I294" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J294" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>32</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr"/>
+      <c r="D295" t="inlineStr"/>
+      <c r="E295" t="inlineStr"/>
+      <c r="F295" t="inlineStr"/>
+      <c r="G295" t="inlineStr"/>
+      <c r="H295" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I295" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J295" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>15</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr"/>
+      <c r="D296" t="inlineStr"/>
+      <c r="E296" t="inlineStr"/>
+      <c r="F296" t="inlineStr"/>
+      <c r="G296" t="inlineStr"/>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I296" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J296" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>8</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr"/>
+      <c r="D297" t="inlineStr"/>
+      <c r="E297" t="inlineStr"/>
+      <c r="F297" t="inlineStr"/>
+      <c r="G297" t="inlineStr"/>
+      <c r="H297" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I297" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J297" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>1</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr"/>
+      <c r="D298" t="inlineStr"/>
+      <c r="E298" t="inlineStr"/>
+      <c r="F298" t="inlineStr"/>
+      <c r="G298" t="inlineStr"/>
+      <c r="H298" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I298" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J298" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>17</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr"/>
+      <c r="D299" t="inlineStr"/>
+      <c r="E299" t="inlineStr"/>
+      <c r="F299" t="inlineStr"/>
+      <c r="G299" t="inlineStr"/>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I299" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J299" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>32</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr"/>
+      <c r="D300" t="inlineStr"/>
+      <c r="E300" t="inlineStr"/>
+      <c r="F300" t="inlineStr"/>
+      <c r="G300" t="inlineStr"/>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I300" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J300" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>23</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr"/>
+      <c r="D301" t="inlineStr"/>
+      <c r="E301" t="inlineStr"/>
+      <c r="F301" t="inlineStr"/>
+      <c r="G301" t="inlineStr"/>
+      <c r="H301" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I301" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J301" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>15</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr"/>
+      <c r="D302" t="inlineStr"/>
+      <c r="E302" t="inlineStr"/>
+      <c r="F302" t="inlineStr"/>
+      <c r="G302" t="inlineStr"/>
+      <c r="H302" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I302" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J302" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>27</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr"/>
+      <c r="D303" t="inlineStr"/>
+      <c r="E303" t="inlineStr"/>
+      <c r="F303" t="inlineStr"/>
+      <c r="G303" t="inlineStr"/>
+      <c r="H303" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I303" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J303" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>28</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr"/>
+      <c r="D304" t="inlineStr"/>
+      <c r="E304" t="inlineStr"/>
+      <c r="F304" t="inlineStr"/>
+      <c r="G304" t="inlineStr"/>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I304" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J304" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>13</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr"/>
+      <c r="D305" t="inlineStr"/>
+      <c r="E305" t="inlineStr"/>
+      <c r="F305" t="inlineStr"/>
+      <c r="G305" t="inlineStr"/>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I305" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J305" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>17</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr"/>
+      <c r="D306" t="inlineStr"/>
+      <c r="E306" t="inlineStr"/>
+      <c r="F306" t="inlineStr"/>
+      <c r="G306" t="inlineStr"/>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I306" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J306" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>15</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr"/>
+      <c r="D307" t="inlineStr"/>
+      <c r="E307" t="inlineStr"/>
+      <c r="F307" t="inlineStr"/>
+      <c r="G307" t="inlineStr"/>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I307" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J307" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>34</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr"/>
+      <c r="D308" t="inlineStr"/>
+      <c r="E308" t="inlineStr"/>
+      <c r="F308" t="inlineStr"/>
+      <c r="G308" t="inlineStr"/>
+      <c r="H308" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I308" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J308" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>35</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr"/>
+      <c r="D309" t="inlineStr"/>
+      <c r="E309" t="inlineStr"/>
+      <c r="F309" t="inlineStr"/>
+      <c r="G309" t="inlineStr"/>
+      <c r="H309" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I309" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J309" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>4</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr"/>
+      <c r="D310" t="inlineStr"/>
+      <c r="E310" t="inlineStr"/>
+      <c r="F310" t="inlineStr"/>
+      <c r="G310" t="inlineStr"/>
+      <c r="H310" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I310" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J310" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>1</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr"/>
+      <c r="D311" t="inlineStr"/>
+      <c r="E311" t="inlineStr"/>
+      <c r="F311" t="inlineStr"/>
+      <c r="G311" t="inlineStr"/>
+      <c r="H311" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I311" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J311" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>34</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr"/>
+      <c r="D312" t="inlineStr"/>
+      <c r="E312" t="inlineStr"/>
+      <c r="F312" t="inlineStr"/>
+      <c r="G312" t="inlineStr"/>
+      <c r="H312" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I312" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J312" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>15</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr"/>
+      <c r="D313" t="inlineStr"/>
+      <c r="E313" t="inlineStr"/>
+      <c r="F313" t="inlineStr"/>
+      <c r="G313" t="inlineStr"/>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I313" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J313" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>19</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr"/>
+      <c r="D314" t="inlineStr"/>
+      <c r="E314" t="inlineStr"/>
+      <c r="F314" t="inlineStr"/>
+      <c r="G314" t="inlineStr"/>
+      <c r="H314" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I314" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J314" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>12</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr"/>
+      <c r="D315" t="inlineStr"/>
+      <c r="E315" t="inlineStr"/>
+      <c r="F315" t="inlineStr"/>
+      <c r="G315" t="inlineStr"/>
+      <c r="H315" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I315" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J315" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>26</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr"/>
+      <c r="D316" t="inlineStr"/>
+      <c r="E316" t="inlineStr"/>
+      <c r="F316" t="inlineStr"/>
+      <c r="G316" t="inlineStr"/>
+      <c r="H316" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I316" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J316" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>9</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr"/>
+      <c r="D317" t="inlineStr"/>
+      <c r="E317" t="inlineStr"/>
+      <c r="F317" t="inlineStr"/>
+      <c r="G317" t="inlineStr"/>
+      <c r="H317" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I317" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J317" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>27</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr"/>
+      <c r="D318" t="inlineStr"/>
+      <c r="E318" t="inlineStr"/>
+      <c r="F318" t="inlineStr"/>
+      <c r="G318" t="inlineStr"/>
+      <c r="H318" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I318" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J318" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>13</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr"/>
+      <c r="D319" t="inlineStr"/>
+      <c r="E319" t="inlineStr"/>
+      <c r="F319" t="inlineStr"/>
+      <c r="G319" t="inlineStr"/>
+      <c r="H319" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I319" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J319" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>5</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr"/>
+      <c r="D320" t="inlineStr"/>
+      <c r="E320" t="inlineStr"/>
+      <c r="F320" t="inlineStr"/>
+      <c r="G320" t="inlineStr"/>
+      <c r="H320" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I320" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J320" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>1</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr"/>
+      <c r="D321" t="inlineStr"/>
+      <c r="E321" t="inlineStr"/>
+      <c r="F321" t="inlineStr"/>
+      <c r="G321" t="inlineStr"/>
+      <c r="H321" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I321" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J321" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>7</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr"/>
+      <c r="D322" t="inlineStr"/>
+      <c r="E322" t="inlineStr"/>
+      <c r="F322" t="inlineStr"/>
+      <c r="G322" t="inlineStr"/>
+      <c r="H322" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I322" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J322" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>5</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr"/>
+      <c r="D323" t="inlineStr"/>
+      <c r="E323" t="inlineStr"/>
+      <c r="F323" t="inlineStr"/>
+      <c r="G323" t="inlineStr"/>
+      <c r="H323" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I323" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J323" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>24</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr"/>
+      <c r="D324" t="inlineStr"/>
+      <c r="E324" t="inlineStr"/>
+      <c r="F324" t="inlineStr"/>
+      <c r="G324" t="inlineStr"/>
+      <c r="H324" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I324" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J324" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>14</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr"/>
+      <c r="D325" t="inlineStr"/>
+      <c r="E325" t="inlineStr"/>
+      <c r="F325" t="inlineStr"/>
+      <c r="G325" t="inlineStr"/>
+      <c r="H325" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I325" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J325" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>20</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr"/>
+      <c r="D326" t="inlineStr"/>
+      <c r="E326" t="inlineStr"/>
+      <c r="F326" t="inlineStr"/>
+      <c r="G326" t="inlineStr"/>
+      <c r="H326" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I326" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J326" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>27</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr"/>
+      <c r="D327" t="inlineStr"/>
+      <c r="E327" t="inlineStr"/>
+      <c r="F327" t="inlineStr"/>
+      <c r="G327" t="inlineStr"/>
+      <c r="H327" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I327" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J327" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>33</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr"/>
+      <c r="D328" t="inlineStr"/>
+      <c r="E328" t="inlineStr"/>
+      <c r="F328" t="inlineStr"/>
+      <c r="G328" t="inlineStr"/>
+      <c r="H328" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I328" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J328" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>16</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr"/>
+      <c r="D329" t="inlineStr"/>
+      <c r="E329" t="inlineStr"/>
+      <c r="F329" t="inlineStr"/>
+      <c r="G329" t="inlineStr"/>
+      <c r="H329" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I329" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J329" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>27</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr"/>
+      <c r="D330" t="inlineStr"/>
+      <c r="E330" t="inlineStr"/>
+      <c r="F330" t="inlineStr"/>
+      <c r="G330" t="inlineStr"/>
+      <c r="H330" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I330" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J330" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>4</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr"/>
+      <c r="D331" t="inlineStr"/>
+      <c r="E331" t="inlineStr"/>
+      <c r="F331" t="inlineStr"/>
+      <c r="G331" t="inlineStr"/>
+      <c r="H331" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I331" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J331" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>27</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr"/>
+      <c r="D332" t="inlineStr"/>
+      <c r="E332" t="inlineStr"/>
+      <c r="F332" t="inlineStr"/>
+      <c r="G332" t="inlineStr"/>
+      <c r="H332" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I332" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J332" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>31</v>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr"/>
+      <c r="D333" t="inlineStr"/>
+      <c r="E333" t="inlineStr"/>
+      <c r="F333" t="inlineStr"/>
+      <c r="G333" t="inlineStr"/>
+      <c r="H333" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I333" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J333" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>13</v>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr"/>
+      <c r="D334" t="inlineStr"/>
+      <c r="E334" t="inlineStr"/>
+      <c r="F334" t="inlineStr"/>
+      <c r="G334" t="inlineStr"/>
+      <c r="H334" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I334" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J334" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>14</v>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr"/>
+      <c r="D335" t="inlineStr"/>
+      <c r="E335" t="inlineStr"/>
+      <c r="F335" t="inlineStr"/>
+      <c r="G335" t="inlineStr"/>
+      <c r="H335" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I335" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J335" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>20</v>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr"/>
+      <c r="D336" t="inlineStr"/>
+      <c r="E336" t="inlineStr"/>
+      <c r="F336" t="inlineStr"/>
+      <c r="G336" t="inlineStr"/>
+      <c r="H336" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I336" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J336" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>7</v>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr"/>
+      <c r="D337" t="inlineStr"/>
+      <c r="E337" t="inlineStr"/>
+      <c r="F337" t="inlineStr"/>
+      <c r="G337" t="inlineStr"/>
+      <c r="H337" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I337" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J337" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>29</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr"/>
+      <c r="D338" t="inlineStr"/>
+      <c r="E338" t="inlineStr"/>
+      <c r="F338" t="inlineStr"/>
+      <c r="G338" t="inlineStr"/>
+      <c r="H338" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I338" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J338" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>16</v>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr"/>
+      <c r="D339" t="inlineStr"/>
+      <c r="E339" t="inlineStr"/>
+      <c r="F339" t="inlineStr"/>
+      <c r="G339" t="inlineStr"/>
+      <c r="H339" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I339" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J339" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>28</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr"/>
+      <c r="D340" t="inlineStr"/>
+      <c r="E340" t="inlineStr"/>
+      <c r="F340" t="inlineStr"/>
+      <c r="G340" t="inlineStr"/>
+      <c r="H340" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I340" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J340" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>32</v>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr"/>
+      <c r="D341" t="inlineStr"/>
+      <c r="E341" t="inlineStr"/>
+      <c r="F341" t="inlineStr"/>
+      <c r="G341" t="inlineStr"/>
+      <c r="H341" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I341" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J341" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>0</v>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr"/>
+      <c r="D342" t="inlineStr"/>
+      <c r="E342" t="inlineStr"/>
+      <c r="F342" t="inlineStr"/>
+      <c r="G342" t="inlineStr"/>
+      <c r="H342" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I342" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J342" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>7</v>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr"/>
+      <c r="D343" t="inlineStr"/>
+      <c r="E343" t="inlineStr"/>
+      <c r="F343" t="inlineStr"/>
+      <c r="G343" t="inlineStr"/>
+      <c r="H343" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I343" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J343" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>5</v>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr"/>
+      <c r="D344" t="inlineStr"/>
+      <c r="E344" t="inlineStr"/>
+      <c r="F344" t="inlineStr"/>
+      <c r="G344" t="inlineStr"/>
+      <c r="H344" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I344" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J344" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>18</v>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr"/>
+      <c r="D345" t="inlineStr"/>
+      <c r="E345" t="inlineStr"/>
+      <c r="F345" t="inlineStr"/>
+      <c r="G345" t="inlineStr"/>
+      <c r="H345" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I345" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J345" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>29</v>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr"/>
+      <c r="D346" t="inlineStr"/>
+      <c r="E346" t="inlineStr"/>
+      <c r="F346" t="inlineStr"/>
+      <c r="G346" t="inlineStr"/>
+      <c r="H346" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I346" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J346" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>34</v>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr"/>
+      <c r="D347" t="inlineStr"/>
+      <c r="E347" t="inlineStr"/>
+      <c r="F347" t="inlineStr"/>
+      <c r="G347" t="inlineStr"/>
+      <c r="H347" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I347" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J347" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>2</v>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr"/>
+      <c r="D348" t="inlineStr"/>
+      <c r="E348" t="inlineStr"/>
+      <c r="F348" t="inlineStr"/>
+      <c r="G348" t="inlineStr"/>
+      <c r="H348" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I348" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J348" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>8</v>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr"/>
+      <c r="D349" t="inlineStr"/>
+      <c r="E349" t="inlineStr"/>
+      <c r="F349" t="inlineStr"/>
+      <c r="G349" t="inlineStr"/>
+      <c r="H349" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I349" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J349" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>11</v>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr"/>
+      <c r="D350" t="inlineStr"/>
+      <c r="E350" t="inlineStr"/>
+      <c r="F350" t="inlineStr"/>
+      <c r="G350" t="inlineStr"/>
+      <c r="H350" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I350" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J350" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>12</v>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr"/>
+      <c r="D351" t="inlineStr"/>
+      <c r="E351" t="inlineStr"/>
+      <c r="F351" t="inlineStr"/>
+      <c r="G351" t="inlineStr"/>
+      <c r="H351" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I351" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J351" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>15</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr"/>
+      <c r="D352" t="inlineStr"/>
+      <c r="E352" t="inlineStr"/>
+      <c r="F352" t="inlineStr"/>
+      <c r="G352" t="inlineStr"/>
+      <c r="H352" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I352" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J352" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>34</v>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr"/>
+      <c r="D353" t="inlineStr"/>
+      <c r="E353" t="inlineStr"/>
+      <c r="F353" t="inlineStr"/>
+      <c r="G353" t="inlineStr"/>
+      <c r="H353" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I353" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J353" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>2</v>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr"/>
+      <c r="D354" t="inlineStr"/>
+      <c r="E354" t="inlineStr"/>
+      <c r="F354" t="inlineStr"/>
+      <c r="G354" t="inlineStr"/>
+      <c r="H354" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I354" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J354" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>33</v>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr"/>
+      <c r="D355" t="inlineStr"/>
+      <c r="E355" t="inlineStr"/>
+      <c r="F355" t="inlineStr"/>
+      <c r="G355" t="inlineStr"/>
+      <c r="H355" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I355" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J355" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>33</v>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr"/>
+      <c r="D356" t="inlineStr"/>
+      <c r="E356" t="inlineStr"/>
+      <c r="F356" t="inlineStr"/>
+      <c r="G356" t="inlineStr"/>
+      <c r="H356" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I356" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J356" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>5</v>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr"/>
+      <c r="D357" t="inlineStr"/>
+      <c r="E357" t="inlineStr"/>
+      <c r="F357" t="inlineStr"/>
+      <c r="G357" t="inlineStr"/>
+      <c r="H357" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I357" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J357" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>1</v>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr"/>
+      <c r="D358" t="inlineStr"/>
+      <c r="E358" t="inlineStr"/>
+      <c r="F358" t="inlineStr"/>
+      <c r="G358" t="inlineStr"/>
+      <c r="H358" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I358" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J358" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>29</v>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr"/>
+      <c r="D359" t="inlineStr"/>
+      <c r="E359" t="inlineStr"/>
+      <c r="F359" t="inlineStr"/>
+      <c r="G359" t="inlineStr"/>
+      <c r="H359" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I359" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J359" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>1</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr"/>
+      <c r="D360" t="inlineStr"/>
+      <c r="E360" t="inlineStr"/>
+      <c r="F360" t="inlineStr"/>
+      <c r="G360" t="inlineStr"/>
+      <c r="H360" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I360" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J360" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>17</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr"/>
+      <c r="D361" t="inlineStr"/>
+      <c r="E361" t="inlineStr"/>
+      <c r="F361" t="inlineStr"/>
+      <c r="G361" t="inlineStr"/>
+      <c r="H361" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I361" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J361" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>10</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr"/>
+      <c r="D362" t="inlineStr"/>
+      <c r="E362" t="inlineStr"/>
+      <c r="F362" t="inlineStr"/>
+      <c r="G362" t="inlineStr"/>
+      <c r="H362" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I362" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J362" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>24</v>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr"/>
+      <c r="D363" t="inlineStr"/>
+      <c r="E363" t="inlineStr"/>
+      <c r="F363" t="inlineStr"/>
+      <c r="G363" t="inlineStr"/>
+      <c r="H363" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I363" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J363" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>21</v>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr"/>
+      <c r="D364" t="inlineStr"/>
+      <c r="E364" t="inlineStr"/>
+      <c r="F364" t="inlineStr"/>
+      <c r="G364" t="inlineStr"/>
+      <c r="H364" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I364" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J364" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>22</v>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr"/>
+      <c r="D365" t="inlineStr"/>
+      <c r="E365" t="inlineStr"/>
+      <c r="F365" t="inlineStr"/>
+      <c r="G365" t="inlineStr"/>
+      <c r="H365" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I365" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J365" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="n">
+        <v>12</v>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr"/>
+      <c r="D366" t="inlineStr"/>
+      <c r="E366" t="inlineStr"/>
+      <c r="F366" t="inlineStr"/>
+      <c r="G366" t="inlineStr"/>
+      <c r="H366" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I366" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J366" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>7</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr"/>
+      <c r="D367" t="inlineStr"/>
+      <c r="E367" t="inlineStr"/>
+      <c r="F367" t="inlineStr"/>
+      <c r="G367" t="inlineStr"/>
+      <c r="H367" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I367" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J367" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="n">
+        <v>18</v>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr"/>
+      <c r="D368" t="inlineStr"/>
+      <c r="E368" t="inlineStr"/>
+      <c r="F368" t="inlineStr"/>
+      <c r="G368" t="inlineStr"/>
+      <c r="H368" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I368" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J368" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="n">
+        <v>3</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr"/>
+      <c r="D369" t="inlineStr"/>
+      <c r="E369" t="inlineStr"/>
+      <c r="F369" t="inlineStr"/>
+      <c r="G369" t="inlineStr"/>
+      <c r="H369" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I369" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J369" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="n">
+        <v>32</v>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr"/>
+      <c r="D370" t="inlineStr"/>
+      <c r="E370" t="inlineStr"/>
+      <c r="F370" t="inlineStr"/>
+      <c r="G370" t="inlineStr"/>
+      <c r="H370" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I370" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J370" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="n">
+        <v>31</v>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr"/>
+      <c r="D371" t="inlineStr"/>
+      <c r="E371" t="inlineStr"/>
+      <c r="F371" t="inlineStr"/>
+      <c r="G371" t="inlineStr"/>
+      <c r="H371" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I371" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J371" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="n">
+        <v>12</v>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr"/>
+      <c r="D372" t="inlineStr"/>
+      <c r="E372" t="inlineStr"/>
+      <c r="F372" t="inlineStr"/>
+      <c r="G372" t="inlineStr"/>
+      <c r="H372" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I372" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J372" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="n">
+        <v>18</v>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr"/>
+      <c r="D373" t="inlineStr"/>
+      <c r="E373" t="inlineStr"/>
+      <c r="F373" t="inlineStr"/>
+      <c r="G373" t="inlineStr"/>
+      <c r="H373" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I373" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J373" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="n">
+        <v>0</v>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr"/>
+      <c r="D374" t="inlineStr"/>
+      <c r="E374" t="inlineStr"/>
+      <c r="F374" t="inlineStr"/>
+      <c r="G374" t="inlineStr"/>
+      <c r="H374" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I374" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J374" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="n">
+        <v>8</v>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr"/>
+      <c r="D375" t="inlineStr"/>
+      <c r="E375" t="inlineStr"/>
+      <c r="F375" t="inlineStr"/>
+      <c r="G375" t="inlineStr"/>
+      <c r="H375" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I375" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J375" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="n">
+        <v>6</v>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr"/>
+      <c r="D376" t="inlineStr"/>
+      <c r="E376" t="inlineStr"/>
+      <c r="F376" t="inlineStr"/>
+      <c r="G376" t="inlineStr"/>
+      <c r="H376" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I376" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J376" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="n">
+        <v>29</v>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr"/>
+      <c r="D377" t="inlineStr"/>
+      <c r="E377" t="inlineStr"/>
+      <c r="F377" t="inlineStr"/>
+      <c r="G377" t="inlineStr"/>
+      <c r="H377" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I377" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J377" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="n">
+        <v>16</v>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr"/>
+      <c r="D378" t="inlineStr"/>
+      <c r="E378" t="inlineStr"/>
+      <c r="F378" t="inlineStr"/>
+      <c r="G378" t="inlineStr"/>
+      <c r="H378" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I378" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J378" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="n">
+        <v>10</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr"/>
+      <c r="D379" t="inlineStr"/>
+      <c r="E379" t="inlineStr"/>
+      <c r="F379" t="inlineStr"/>
+      <c r="G379" t="inlineStr"/>
+      <c r="H379" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I379" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J379" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="n">
+        <v>15</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr"/>
+      <c r="D380" t="inlineStr"/>
+      <c r="E380" t="inlineStr"/>
+      <c r="F380" t="inlineStr"/>
+      <c r="G380" t="inlineStr"/>
+      <c r="H380" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I380" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J380" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="n">
+        <v>4</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr"/>
+      <c r="D381" t="inlineStr"/>
+      <c r="E381" t="inlineStr"/>
+      <c r="F381" t="inlineStr"/>
+      <c r="G381" t="inlineStr"/>
+      <c r="H381" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I381" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J381" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="n">
+        <v>3</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr"/>
+      <c r="D382" t="inlineStr"/>
+      <c r="E382" t="inlineStr"/>
+      <c r="F382" t="inlineStr"/>
+      <c r="G382" t="inlineStr"/>
+      <c r="H382" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I382" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J382" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="n">
+        <v>20</v>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr"/>
+      <c r="D383" t="inlineStr"/>
+      <c r="E383" t="inlineStr"/>
+      <c r="F383" t="inlineStr"/>
+      <c r="G383" t="inlineStr"/>
+      <c r="H383" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I383" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J383" t="n">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="n">
+        <v>22</v>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr"/>
+      <c r="D384" t="inlineStr"/>
+      <c r="E384" t="inlineStr"/>
+      <c r="F384" t="inlineStr"/>
+      <c r="G384" t="inlineStr"/>
+      <c r="H384" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I384" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J384" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>17</v>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr"/>
+      <c r="D385" t="inlineStr"/>
+      <c r="E385" t="inlineStr"/>
+      <c r="F385" t="inlineStr"/>
+      <c r="G385" t="inlineStr"/>
+      <c r="H385" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I385" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J385" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>16</v>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr"/>
+      <c r="D386" t="inlineStr"/>
+      <c r="E386" t="inlineStr"/>
+      <c r="F386" t="inlineStr"/>
+      <c r="G386" t="inlineStr"/>
+      <c r="H386" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I386" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J386" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n">
+        <v>5</v>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr"/>
+      <c r="D387" t="inlineStr"/>
+      <c r="E387" t="inlineStr"/>
+      <c r="F387" t="inlineStr"/>
+      <c r="G387" t="inlineStr"/>
+      <c r="H387" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I387" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J387" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="n">
+        <v>19</v>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr"/>
+      <c r="D388" t="inlineStr"/>
+      <c r="E388" t="inlineStr"/>
+      <c r="F388" t="inlineStr"/>
+      <c r="G388" t="inlineStr"/>
+      <c r="H388" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I388" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J388" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="n">
+        <v>16</v>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr"/>
+      <c r="D389" t="inlineStr"/>
+      <c r="E389" t="inlineStr"/>
+      <c r="F389" t="inlineStr"/>
+      <c r="G389" t="inlineStr"/>
+      <c r="H389" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I389" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J389" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="n">
+        <v>0</v>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr"/>
+      <c r="D390" t="inlineStr"/>
+      <c r="E390" t="inlineStr"/>
+      <c r="F390" t="inlineStr"/>
+      <c r="G390" t="inlineStr"/>
+      <c r="H390" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I390" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J390" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="n">
+        <v>8</v>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr"/>
+      <c r="D391" t="inlineStr"/>
+      <c r="E391" t="inlineStr"/>
+      <c r="F391" t="inlineStr"/>
+      <c r="G391" t="inlineStr"/>
+      <c r="H391" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I391" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J391" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n">
+        <v>28</v>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr"/>
+      <c r="D392" t="inlineStr"/>
+      <c r="E392" t="inlineStr"/>
+      <c r="F392" t="inlineStr"/>
+      <c r="G392" t="inlineStr"/>
+      <c r="H392" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I392" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J392" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="n">
+        <v>12</v>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr"/>
+      <c r="D393" t="inlineStr"/>
+      <c r="E393" t="inlineStr"/>
+      <c r="F393" t="inlineStr"/>
+      <c r="G393" t="inlineStr"/>
+      <c r="H393" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I393" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J393" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="n">
+        <v>33</v>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr"/>
+      <c r="D394" t="inlineStr"/>
+      <c r="E394" t="inlineStr"/>
+      <c r="F394" t="inlineStr"/>
+      <c r="G394" t="inlineStr"/>
+      <c r="H394" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I394" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J394" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="n">
+        <v>3</v>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr"/>
+      <c r="D395" t="inlineStr"/>
+      <c r="E395" t="inlineStr"/>
+      <c r="F395" t="inlineStr"/>
+      <c r="G395" t="inlineStr"/>
+      <c r="H395" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I395" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J395" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="n">
+        <v>22</v>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr"/>
+      <c r="D396" t="inlineStr"/>
+      <c r="E396" t="inlineStr"/>
+      <c r="F396" t="inlineStr"/>
+      <c r="G396" t="inlineStr"/>
+      <c r="H396" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I396" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J396" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="n">
+        <v>29</v>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr"/>
+      <c r="D397" t="inlineStr"/>
+      <c r="E397" t="inlineStr"/>
+      <c r="F397" t="inlineStr"/>
+      <c r="G397" t="inlineStr"/>
+      <c r="H397" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I397" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J397" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="n">
+        <v>21</v>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr"/>
+      <c r="D398" t="inlineStr"/>
+      <c r="E398" t="inlineStr"/>
+      <c r="F398" t="inlineStr"/>
+      <c r="G398" t="inlineStr"/>
+      <c r="H398" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I398" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J398" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="n">
+        <v>31</v>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr"/>
+      <c r="D399" t="inlineStr"/>
+      <c r="E399" t="inlineStr"/>
+      <c r="F399" t="inlineStr"/>
+      <c r="G399" t="inlineStr"/>
+      <c r="H399" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I399" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J399" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="n">
+        <v>35</v>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr"/>
+      <c r="D400" t="inlineStr"/>
+      <c r="E400" t="inlineStr"/>
+      <c r="F400" t="inlineStr"/>
+      <c r="G400" t="inlineStr"/>
+      <c r="H400" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I400" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J400" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="n">
+        <v>13</v>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr"/>
+      <c r="D401" t="inlineStr"/>
+      <c r="E401" t="inlineStr"/>
+      <c r="F401" t="inlineStr"/>
+      <c r="G401" t="inlineStr"/>
+      <c r="H401" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I401" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J401" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="n">
+        <v>36</v>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr"/>
+      <c r="D402" t="inlineStr"/>
+      <c r="E402" t="inlineStr"/>
+      <c r="F402" t="inlineStr"/>
+      <c r="G402" t="inlineStr"/>
+      <c r="H402" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I402" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J402" t="n">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="n">
+        <v>6</v>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr"/>
+      <c r="D403" t="inlineStr"/>
+      <c r="E403" t="inlineStr"/>
+      <c r="F403" t="inlineStr"/>
+      <c r="G403" t="inlineStr"/>
+      <c r="H403" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I403" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J403" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="n">
+        <v>23</v>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr"/>
+      <c r="D404" t="inlineStr"/>
+      <c r="E404" t="inlineStr"/>
+      <c r="F404" t="inlineStr"/>
+      <c r="G404" t="inlineStr"/>
+      <c r="H404" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I404" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J404" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="n">
+        <v>26</v>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr"/>
+      <c r="D405" t="inlineStr"/>
+      <c r="E405" t="inlineStr"/>
+      <c r="F405" t="inlineStr"/>
+      <c r="G405" t="inlineStr"/>
+      <c r="H405" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I405" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J405" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="n">
+        <v>9</v>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr"/>
+      <c r="D406" t="inlineStr"/>
+      <c r="E406" t="inlineStr"/>
+      <c r="F406" t="inlineStr"/>
+      <c r="G406" t="inlineStr"/>
+      <c r="H406" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I406" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J406" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="n">
+        <v>29</v>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr"/>
+      <c r="D407" t="inlineStr"/>
+      <c r="E407" t="inlineStr"/>
+      <c r="F407" t="inlineStr"/>
+      <c r="G407" t="inlineStr"/>
+      <c r="H407" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I407" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J407" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="n">
+        <v>28</v>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr"/>
+      <c r="D408" t="inlineStr"/>
+      <c r="E408" t="inlineStr"/>
+      <c r="F408" t="inlineStr"/>
+      <c r="G408" t="inlineStr"/>
+      <c r="H408" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I408" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J408" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="n">
+        <v>35</v>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr"/>
+      <c r="D409" t="inlineStr"/>
+      <c r="E409" t="inlineStr"/>
+      <c r="F409" t="inlineStr"/>
+      <c r="G409" t="inlineStr"/>
+      <c r="H409" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I409" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J409" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="n">
+        <v>27</v>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr"/>
+      <c r="D410" t="inlineStr"/>
+      <c r="E410" t="inlineStr"/>
+      <c r="F410" t="inlineStr"/>
+      <c r="G410" t="inlineStr"/>
+      <c r="H410" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I410" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J410" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="n">
+        <v>28</v>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr"/>
+      <c r="D411" t="inlineStr"/>
+      <c r="E411" t="inlineStr"/>
+      <c r="F411" t="inlineStr"/>
+      <c r="G411" t="inlineStr"/>
+      <c r="H411" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I411" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J411" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="n">
+        <v>17</v>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr"/>
+      <c r="D412" t="inlineStr"/>
+      <c r="E412" t="inlineStr"/>
+      <c r="F412" t="inlineStr"/>
+      <c r="G412" t="inlineStr"/>
+      <c r="H412" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I412" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J412" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="n">
+        <v>10</v>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr"/>
+      <c r="D413" t="inlineStr"/>
+      <c r="E413" t="inlineStr"/>
+      <c r="F413" t="inlineStr"/>
+      <c r="G413" t="inlineStr"/>
+      <c r="H413" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I413" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J413" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="n">
+        <v>18</v>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr"/>
+      <c r="D414" t="inlineStr"/>
+      <c r="E414" t="inlineStr"/>
+      <c r="F414" t="inlineStr"/>
+      <c r="G414" t="inlineStr"/>
+      <c r="H414" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I414" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J414" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="n">
+        <v>13</v>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr"/>
+      <c r="D415" t="inlineStr"/>
+      <c r="E415" t="inlineStr"/>
+      <c r="F415" t="inlineStr"/>
+      <c r="G415" t="inlineStr"/>
+      <c r="H415" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I415" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J415" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="n">
+        <v>7</v>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr"/>
+      <c r="D416" t="inlineStr"/>
+      <c r="E416" t="inlineStr"/>
+      <c r="F416" t="inlineStr"/>
+      <c r="G416" t="inlineStr"/>
+      <c r="H416" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I416" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J416" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="n">
+        <v>25</v>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr"/>
+      <c r="D417" t="inlineStr"/>
+      <c r="E417" t="inlineStr"/>
+      <c r="F417" t="inlineStr"/>
+      <c r="G417" t="inlineStr"/>
+      <c r="H417" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I417" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J417" t="n">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="n">
+        <v>8</v>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr"/>
+      <c r="D418" t="inlineStr"/>
+      <c r="E418" t="inlineStr"/>
+      <c r="F418" t="inlineStr"/>
+      <c r="G418" t="inlineStr"/>
+      <c r="H418" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I418" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J418" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="n">
+        <v>16</v>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr"/>
+      <c r="D419" t="inlineStr"/>
+      <c r="E419" t="inlineStr"/>
+      <c r="F419" t="inlineStr"/>
+      <c r="G419" t="inlineStr"/>
+      <c r="H419" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I419" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J419" t="n">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="n">
+        <v>33</v>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr"/>
+      <c r="D420" t="inlineStr"/>
+      <c r="E420" t="inlineStr"/>
+      <c r="F420" t="inlineStr"/>
+      <c r="G420" t="inlineStr"/>
+      <c r="H420" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I420" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J420" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="n">
+        <v>17</v>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr"/>
+      <c r="D421" t="inlineStr"/>
+      <c r="E421" t="inlineStr"/>
+      <c r="F421" t="inlineStr"/>
+      <c r="G421" t="inlineStr"/>
+      <c r="H421" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I421" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J421" t="n">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="n">
+        <v>6</v>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr"/>
+      <c r="D422" t="inlineStr"/>
+      <c r="E422" t="inlineStr"/>
+      <c r="F422" t="inlineStr"/>
+      <c r="G422" t="inlineStr"/>
+      <c r="H422" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I422" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J422" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="n">
+        <v>15</v>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr"/>
+      <c r="D423" t="inlineStr"/>
+      <c r="E423" t="inlineStr"/>
+      <c r="F423" t="inlineStr"/>
+      <c r="G423" t="inlineStr"/>
+      <c r="H423" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I423" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J423" t="n">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="n">
+        <v>35</v>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr"/>
+      <c r="D424" t="inlineStr"/>
+      <c r="E424" t="inlineStr"/>
+      <c r="F424" t="inlineStr"/>
+      <c r="G424" t="inlineStr"/>
+      <c r="H424" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I424" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J424" t="n">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="n">
+        <v>3</v>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr"/>
+      <c r="D425" t="inlineStr"/>
+      <c r="E425" t="inlineStr"/>
+      <c r="F425" t="inlineStr"/>
+      <c r="G425" t="inlineStr"/>
+      <c r="H425" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I425" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J425" t="n">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="n">
+        <v>26</v>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr"/>
+      <c r="D426" t="inlineStr"/>
+      <c r="E426" t="inlineStr"/>
+      <c r="F426" t="inlineStr"/>
+      <c r="G426" t="inlineStr"/>
+      <c r="H426" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I426" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J426" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="n">
+        <v>4</v>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr"/>
+      <c r="D427" t="inlineStr"/>
+      <c r="E427" t="inlineStr"/>
+      <c r="F427" t="inlineStr"/>
+      <c r="G427" t="inlineStr"/>
+      <c r="H427" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I427" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J427" t="n">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="n">
+        <v>7</v>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr"/>
+      <c r="D428" t="inlineStr"/>
+      <c r="E428" t="inlineStr"/>
+      <c r="F428" t="inlineStr"/>
+      <c r="G428" t="inlineStr"/>
+      <c r="H428" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I428" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J428" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="n">
+        <v>29</v>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr"/>
+      <c r="D429" t="inlineStr"/>
+      <c r="E429" t="inlineStr"/>
+      <c r="F429" t="inlineStr"/>
+      <c r="G429" t="inlineStr"/>
+      <c r="H429" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I429" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J429" t="n">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="n">
+        <v>26</v>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr"/>
+      <c r="D430" t="inlineStr"/>
+      <c r="E430" t="inlineStr"/>
+      <c r="F430" t="inlineStr"/>
+      <c r="G430" t="inlineStr"/>
+      <c r="H430" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I430" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J430" t="n">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>